<commit_message>
temporary fix for references
</commit_message>
<xml_diff>
--- a/comma.xlsx
+++ b/comma.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="TämäTyökirja" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\HESSO\excelfiles\testexcelthing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonathan.albrecht\Documents\GitHub\SGTRI_2.0_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0B0F2A-1BB2-4C8D-BBCF-9129FB59B4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A254FC76-5016-4A36-B32E-44FEE6126300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{E45F45C2-6DB2-438B-9E6A-51AA33F5D261}"/>
+    <workbookView xWindow="60285" yWindow="3870" windowWidth="28800" windowHeight="15375" xr2:uid="{E45F45C2-6DB2-438B-9E6A-51AA33F5D261}"/>
   </bookViews>
   <sheets>
     <sheet name="qswithtags" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11206" uniqueCount="1689">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11206" uniqueCount="1694">
   <si>
     <t>No_Controle</t>
   </si>
@@ -5115,13 +5115,28 @@
   </si>
   <si>
     <t>Ingestion pile/aimant/objet tranchant</t>
+  </si>
+  <si>
+    <t>V32</t>
+  </si>
+  <si>
+    <t>V33</t>
+  </si>
+  <si>
+    <t>V34</t>
+  </si>
+  <si>
+    <t>V35</t>
+  </si>
+  <si>
+    <t>V36</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5147,6 +5162,12 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -5253,8 +5274,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normaali" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 40" xfId="1" xr:uid="{BF9C5DFE-9E07-46D6-9E99-7D183E3F2491}"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="78">
     <dxf>
@@ -5587,39 +5608,39 @@
     <tableColumn id="5" xr3:uid="{1BF16328-E2DC-4D41-9B4B-2618046FCCE4}" uniqueName="5" name="V1" queryTableFieldId="5" dataDxfId="75"/>
     <tableColumn id="6" xr3:uid="{4EF86385-418C-4EEB-9DFF-8EF90C3061A6}" uniqueName="6" name="V2" queryTableFieldId="6" dataDxfId="74"/>
     <tableColumn id="7" xr3:uid="{5291B92A-D9BB-4994-A511-829A6FABC345}" uniqueName="7" name="V3" queryTableFieldId="7" dataDxfId="73"/>
-    <tableColumn id="8" xr3:uid="{B8AF0813-353B-443F-98EA-17BAB20AB546}" uniqueName="8" name="V1A" queryTableFieldId="8" dataDxfId="72"/>
-    <tableColumn id="9" xr3:uid="{9C03F574-BBF3-40A3-B54A-3CE39D971FB5}" uniqueName="9" name="V4" queryTableFieldId="9" dataDxfId="71"/>
-    <tableColumn id="10" xr3:uid="{14D0925F-1547-4809-8995-1577CE8F3967}" uniqueName="10" name="V4A" queryTableFieldId="10" dataDxfId="70"/>
-    <tableColumn id="11" xr3:uid="{B9CCEB1C-C860-4117-8C59-D5CB2AA498FA}" uniqueName="11" name="V5" queryTableFieldId="11" dataDxfId="69"/>
-    <tableColumn id="12" xr3:uid="{67353817-B463-480A-A470-93A0828B6C9E}" uniqueName="12" name="V6" queryTableFieldId="12" dataDxfId="68"/>
-    <tableColumn id="13" xr3:uid="{17554286-479F-4059-9555-B93545EAA875}" uniqueName="13" name="V7" queryTableFieldId="13" dataDxfId="67"/>
-    <tableColumn id="14" xr3:uid="{65031D24-641C-4617-AC1B-D32F1E6A858E}" uniqueName="14" name="V8" queryTableFieldId="14" dataDxfId="66"/>
-    <tableColumn id="15" xr3:uid="{3D1D4A39-5606-4340-8B45-25A18B766DA2}" uniqueName="15" name="V9" queryTableFieldId="15" dataDxfId="65"/>
-    <tableColumn id="16" xr3:uid="{D35468A3-DAE6-4E63-BCD4-F2D7D09EF1C8}" uniqueName="16" name="V10" queryTableFieldId="16" dataDxfId="64"/>
-    <tableColumn id="17" xr3:uid="{1D2FAB31-077D-4337-A038-C418876DAFD5}" uniqueName="17" name="V11" queryTableFieldId="17" dataDxfId="63"/>
-    <tableColumn id="18" xr3:uid="{F77AA3A1-7388-4953-9F66-6BD18477324A}" uniqueName="18" name="V12" queryTableFieldId="18" dataDxfId="62"/>
-    <tableColumn id="19" xr3:uid="{BDD0CC5F-AE70-4CFD-89AB-E19ED670396B}" uniqueName="19" name="V13" queryTableFieldId="19" dataDxfId="61"/>
-    <tableColumn id="20" xr3:uid="{592B6D19-DE0F-4263-80A5-3662FB94E2F2}" uniqueName="20" name="V14" queryTableFieldId="20" dataDxfId="60"/>
-    <tableColumn id="21" xr3:uid="{B6E55AFA-4475-4820-81C9-66CBAF8B7469}" uniqueName="21" name="V15" queryTableFieldId="21" dataDxfId="59"/>
-    <tableColumn id="22" xr3:uid="{7A18346F-A1FA-41ED-A3B1-1B9404A9B0FE}" uniqueName="22" name="V16" queryTableFieldId="22" dataDxfId="58"/>
-    <tableColumn id="23" xr3:uid="{778CFB67-6CED-47BE-AD7A-3E8767A533E8}" uniqueName="23" name="V17" queryTableFieldId="23" dataDxfId="57"/>
-    <tableColumn id="24" xr3:uid="{68FCAF3F-8304-4E7B-9DC8-BCC6E52EC855}" uniqueName="24" name="V5A" queryTableFieldId="24" dataDxfId="56"/>
-    <tableColumn id="25" xr3:uid="{D6BB44FE-A28D-45D3-B39F-7900F6DF7598}" uniqueName="25" name="V18" queryTableFieldId="25" dataDxfId="55"/>
-    <tableColumn id="26" xr3:uid="{EFFA2C15-DA36-40A1-9756-D040DC2AB01B}" uniqueName="26" name="V19" queryTableFieldId="26" dataDxfId="54"/>
-    <tableColumn id="27" xr3:uid="{2DE66529-CC53-40FD-AAB4-604849809336}" uniqueName="27" name="V20" queryTableFieldId="27" dataDxfId="53"/>
-    <tableColumn id="28" xr3:uid="{9C415832-A277-4CCE-9E18-B91E706B4AB4}" uniqueName="28" name="Column1" queryTableFieldId="28" dataDxfId="52"/>
-    <tableColumn id="29" xr3:uid="{319E079C-A43B-49BA-A536-11D0EAA46F12}" uniqueName="29" name="V21" queryTableFieldId="29" dataDxfId="51"/>
-    <tableColumn id="30" xr3:uid="{B97E009C-8ADB-474F-A60F-D479B5D65F60}" uniqueName="30" name="V22" queryTableFieldId="30" dataDxfId="50"/>
-    <tableColumn id="31" xr3:uid="{7B615CB9-981F-44D9-95CE-2BC360DE7E31}" uniqueName="31" name="V23" queryTableFieldId="31" dataDxfId="49"/>
-    <tableColumn id="32" xr3:uid="{C966F225-D806-45EF-BDBE-D90D71E39BE5}" uniqueName="32" name="V24" queryTableFieldId="32" dataDxfId="48"/>
-    <tableColumn id="33" xr3:uid="{F4E3F5EB-8078-46FE-8D3D-10BB265C76BE}" uniqueName="33" name="V25" queryTableFieldId="33" dataDxfId="47"/>
-    <tableColumn id="34" xr3:uid="{F81A1E36-4BE9-4225-9CBC-90D4ABA95A79}" uniqueName="34" name="V26" queryTableFieldId="34" dataDxfId="46"/>
-    <tableColumn id="35" xr3:uid="{E354C692-4C9E-4EE2-BCCD-7D84DA143BED}" uniqueName="35" name="V27" queryTableFieldId="35" dataDxfId="45"/>
-    <tableColumn id="36" xr3:uid="{2A0A9041-800F-43A0-B1CF-C05E4402172B}" uniqueName="36" name="V28" queryTableFieldId="36" dataDxfId="44"/>
-    <tableColumn id="37" xr3:uid="{F8BDA19D-9C0B-4351-A8D4-5245F8FD6FB9}" uniqueName="37" name="V29" queryTableFieldId="37" dataDxfId="43"/>
-    <tableColumn id="38" xr3:uid="{364164A4-57E5-4393-AA87-FA9DB02FB864}" uniqueName="38" name="V30" queryTableFieldId="38" dataDxfId="42"/>
-    <tableColumn id="39" xr3:uid="{EEABB42E-1F79-44E1-BF87-A928A2DC1C4C}" uniqueName="39" name="V31" queryTableFieldId="39" dataDxfId="41"/>
-    <tableColumn id="40" xr3:uid="{E7F14C57-F620-46D2-9084-A282A6B5B7DC}" uniqueName="40" name="VA21 " queryTableFieldId="40" dataDxfId="40"/>
+    <tableColumn id="8" xr3:uid="{B8AF0813-353B-443F-98EA-17BAB20AB546}" uniqueName="8" name="V4" queryTableFieldId="8" dataDxfId="72"/>
+    <tableColumn id="9" xr3:uid="{9C03F574-BBF3-40A3-B54A-3CE39D971FB5}" uniqueName="9" name="V5" queryTableFieldId="9" dataDxfId="71"/>
+    <tableColumn id="10" xr3:uid="{14D0925F-1547-4809-8995-1577CE8F3967}" uniqueName="10" name="V6" queryTableFieldId="10" dataDxfId="70"/>
+    <tableColumn id="11" xr3:uid="{B9CCEB1C-C860-4117-8C59-D5CB2AA498FA}" uniqueName="11" name="V7" queryTableFieldId="11" dataDxfId="69"/>
+    <tableColumn id="12" xr3:uid="{67353817-B463-480A-A470-93A0828B6C9E}" uniqueName="12" name="V8" queryTableFieldId="12" dataDxfId="68"/>
+    <tableColumn id="13" xr3:uid="{17554286-479F-4059-9555-B93545EAA875}" uniqueName="13" name="V9" queryTableFieldId="13" dataDxfId="67"/>
+    <tableColumn id="14" xr3:uid="{65031D24-641C-4617-AC1B-D32F1E6A858E}" uniqueName="14" name="V10" queryTableFieldId="14" dataDxfId="66"/>
+    <tableColumn id="15" xr3:uid="{3D1D4A39-5606-4340-8B45-25A18B766DA2}" uniqueName="15" name="V11" queryTableFieldId="15" dataDxfId="65"/>
+    <tableColumn id="16" xr3:uid="{D35468A3-DAE6-4E63-BCD4-F2D7D09EF1C8}" uniqueName="16" name="V12" queryTableFieldId="16" dataDxfId="64"/>
+    <tableColumn id="17" xr3:uid="{1D2FAB31-077D-4337-A038-C418876DAFD5}" uniqueName="17" name="V13" queryTableFieldId="17" dataDxfId="63"/>
+    <tableColumn id="18" xr3:uid="{F77AA3A1-7388-4953-9F66-6BD18477324A}" uniqueName="18" name="V14" queryTableFieldId="18" dataDxfId="62"/>
+    <tableColumn id="19" xr3:uid="{BDD0CC5F-AE70-4CFD-89AB-E19ED670396B}" uniqueName="19" name="V15" queryTableFieldId="19" dataDxfId="61"/>
+    <tableColumn id="20" xr3:uid="{592B6D19-DE0F-4263-80A5-3662FB94E2F2}" uniqueName="20" name="V16" queryTableFieldId="20" dataDxfId="60"/>
+    <tableColumn id="21" xr3:uid="{B6E55AFA-4475-4820-81C9-66CBAF8B7469}" uniqueName="21" name="V17" queryTableFieldId="21" dataDxfId="59"/>
+    <tableColumn id="22" xr3:uid="{7A18346F-A1FA-41ED-A3B1-1B9404A9B0FE}" uniqueName="22" name="V18" queryTableFieldId="22" dataDxfId="58"/>
+    <tableColumn id="23" xr3:uid="{778CFB67-6CED-47BE-AD7A-3E8767A533E8}" uniqueName="23" name="V19" queryTableFieldId="23" dataDxfId="57"/>
+    <tableColumn id="24" xr3:uid="{68FCAF3F-8304-4E7B-9DC8-BCC6E52EC855}" uniqueName="24" name="V20" queryTableFieldId="24" dataDxfId="56"/>
+    <tableColumn id="25" xr3:uid="{D6BB44FE-A28D-45D3-B39F-7900F6DF7598}" uniqueName="25" name="V21" queryTableFieldId="25" dataDxfId="55"/>
+    <tableColumn id="26" xr3:uid="{EFFA2C15-DA36-40A1-9756-D040DC2AB01B}" uniqueName="26" name="V22" queryTableFieldId="26" dataDxfId="54"/>
+    <tableColumn id="27" xr3:uid="{2DE66529-CC53-40FD-AAB4-604849809336}" uniqueName="27" name="V23" queryTableFieldId="27" dataDxfId="53"/>
+    <tableColumn id="28" xr3:uid="{9C415832-A277-4CCE-9E18-B91E706B4AB4}" uniqueName="28" name="V24" queryTableFieldId="28" dataDxfId="52"/>
+    <tableColumn id="29" xr3:uid="{319E079C-A43B-49BA-A536-11D0EAA46F12}" uniqueName="29" name="V25" queryTableFieldId="29" dataDxfId="51"/>
+    <tableColumn id="30" xr3:uid="{B97E009C-8ADB-474F-A60F-D479B5D65F60}" uniqueName="30" name="V26" queryTableFieldId="30" dataDxfId="50"/>
+    <tableColumn id="31" xr3:uid="{7B615CB9-981F-44D9-95CE-2BC360DE7E31}" uniqueName="31" name="V27" queryTableFieldId="31" dataDxfId="49"/>
+    <tableColumn id="32" xr3:uid="{C966F225-D806-45EF-BDBE-D90D71E39BE5}" uniqueName="32" name="V28" queryTableFieldId="32" dataDxfId="48"/>
+    <tableColumn id="33" xr3:uid="{F4E3F5EB-8078-46FE-8D3D-10BB265C76BE}" uniqueName="33" name="V29" queryTableFieldId="33" dataDxfId="47"/>
+    <tableColumn id="34" xr3:uid="{F81A1E36-4BE9-4225-9CBC-90D4ABA95A79}" uniqueName="34" name="V30" queryTableFieldId="34" dataDxfId="46"/>
+    <tableColumn id="35" xr3:uid="{E354C692-4C9E-4EE2-BCCD-7D84DA143BED}" uniqueName="35" name="V31" queryTableFieldId="35" dataDxfId="45"/>
+    <tableColumn id="36" xr3:uid="{2A0A9041-800F-43A0-B1CF-C05E4402172B}" uniqueName="36" name="V32" queryTableFieldId="36" dataDxfId="44"/>
+    <tableColumn id="37" xr3:uid="{F8BDA19D-9C0B-4351-A8D4-5245F8FD6FB9}" uniqueName="37" name="V33" queryTableFieldId="37" dataDxfId="43"/>
+    <tableColumn id="38" xr3:uid="{364164A4-57E5-4393-AA87-FA9DB02FB864}" uniqueName="38" name="V34" queryTableFieldId="38" dataDxfId="42"/>
+    <tableColumn id="39" xr3:uid="{EEABB42E-1F79-44E1-BF87-A928A2DC1C4C}" uniqueName="39" name="V35" queryTableFieldId="39" dataDxfId="41"/>
+    <tableColumn id="40" xr3:uid="{E7F14C57-F620-46D2-9084-A282A6B5B7DC}" uniqueName="40" name="V36" queryTableFieldId="40" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5676,7 +5697,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-teema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5975,11 +5996,11 @@
   <sheetPr codeName="Taul1"/>
   <dimension ref="A1:AM138"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="39" width="80.7265625" bestFit="1" customWidth="1"/>
@@ -6005,103 +6026,103 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="H1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="L1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="P1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="Q1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="R1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="S1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="T1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="U1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="V1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="W1" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="X1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="Y1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="Z1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="AA1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="AB1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="AC1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="AD1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="AE1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="AF1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="AG1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="AH1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="AI1" t="s">
-        <v>34</v>
+        <v>1689</v>
       </c>
       <c r="AJ1" t="s">
-        <v>35</v>
+        <v>1690</v>
       </c>
       <c r="AK1" t="s">
-        <v>36</v>
+        <v>1691</v>
       </c>
       <c r="AL1" t="s">
-        <v>37</v>
+        <v>1692</v>
       </c>
       <c r="AM1" t="s">
-        <v>38</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="2" spans="1:39" x14ac:dyDescent="0.35">
@@ -22408,6 +22429,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -22420,11 +22442,11 @@
   <sheetPr codeName="Taul3"/>
   <dimension ref="A1:AN181"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13.36328125" customWidth="1"/>
     <col min="2" max="2" width="45.7265625" customWidth="1"/>
@@ -42178,7 +42200,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="4" max="4" width="55.36328125" customWidth="1"/>

</xml_diff>